<commit_message>
changed the names in the data
</commit_message>
<xml_diff>
--- a/SummerAvailabilityWeek7.xlsx
+++ b/SummerAvailabilityWeek7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pelumi\Documents\GeneticScheduler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pelumi\SideProjects\GeneticScheduler2.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44660293-6C57-4D14-B4EB-1223AF246C5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B982250-0683-4441-AB18-9DD8673D81AD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{DE2743BD-8EF0-4AC6-864B-9589428D9021}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{DE2743BD-8EF0-4AC6-864B-9589428D9021}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -195,9 +195,6 @@
     <t>Friday (6/28) [4:55 pm - close]</t>
   </si>
   <si>
-    <t>Elizabeth Hergert</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -219,49 +216,52 @@
     <t>I WANT to work this shift</t>
   </si>
   <si>
-    <t>Alyson</t>
-  </si>
-  <si>
     <t>2 hours</t>
   </si>
   <si>
-    <t>Adriana Amaris</t>
-  </si>
-  <si>
-    <t>sarah gao</t>
-  </si>
-  <si>
-    <t>marlena fleck</t>
-  </si>
-  <si>
     <t>Gabby</t>
   </si>
   <si>
     <t>3 hours, 4 hours</t>
   </si>
   <si>
-    <t>nina</t>
-  </si>
-  <si>
-    <t>Andrea Doan</t>
-  </si>
-  <si>
-    <t>Miguel</t>
-  </si>
-  <si>
-    <t>Laura Jabr</t>
-  </si>
-  <si>
-    <t>Alex</t>
-  </si>
-  <si>
     <t>3 hours</t>
   </si>
   <si>
-    <t>Morgan Seay</t>
-  </si>
-  <si>
-    <t>Leo</t>
+    <t>Eli</t>
+  </si>
+  <si>
+    <t>Aaron</t>
+  </si>
+  <si>
+    <t>Adrian</t>
+  </si>
+  <si>
+    <t>Leonard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Morgan </t>
+  </si>
+  <si>
+    <t>Allen</t>
+  </si>
+  <si>
+    <t>Ayomide</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Ngozi</t>
+  </si>
+  <si>
+    <t>Saeda</t>
+  </si>
+  <si>
+    <t>Modupe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leena </t>
   </si>
 </sst>
 </file>
@@ -269,7 +269,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0;[Red]0"/>
+    <numFmt numFmtId="164" formatCode="0;[Red]0"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -374,7 +374,7 @@
     <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -693,8 +693,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92AEFEBE-42DE-4ACA-9400-A6D85B11D141}">
   <dimension ref="A1:BB14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -865,2134 +865,2134 @@
     </row>
     <row r="2" spans="1:54" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="D2" s="3">
         <v>15</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="W2" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="X2" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Y2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z2" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AG2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AJ2" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AK2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AN2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AO2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AP2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AQ2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AR2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AS2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AT2" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AU2" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AV2" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AW2" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AX2" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AY2" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AZ2" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="BA2" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BB2" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:54" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D3" s="3">
         <v>11</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="S3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="T3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="V3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="X3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Z3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AB3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AC3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AE3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AF3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AG3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AH3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AI3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AJ3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AK3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AL3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AM3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AN3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AO3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AP3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AQ3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AR3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AS3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AT3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AU3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AV3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AW3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AX3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AY3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AZ3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BA3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BB3" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:54" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D4" s="3">
         <v>10</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="V4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AB4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AC4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AD4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AE4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AF4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AG4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AL4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AM4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AN4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AO4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AP4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AQ4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AR4" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AS4" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AT4" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AU4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AV4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AW4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AX4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AY4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AZ4" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="BA4" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BB4" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:54" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="D5" s="8">
         <v>9</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="V5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="X5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Y5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AC5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AD5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AE5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AF5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AG5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AH5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AI5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AM5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AN5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AO5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AP5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AQ5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AR5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AS5" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AT5" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AU5" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AV5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AW5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AX5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AY5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AZ5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="BA5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="BB5" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:54" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D6" s="3">
         <v>12</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="V6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="X6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Y6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Z6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AB6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AC6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AD6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AJ6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AK6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AL6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AM6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AN6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AO6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AP6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AQ6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AR6" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AS6" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AT6" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AU6" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AV6" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AW6" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AX6" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AY6" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AZ6" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BA6" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BB6" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:54" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D7" s="3">
         <v>12</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N7" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="O7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="P7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Q7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="S7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="T7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="U7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="V7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="X7" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Y7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Z7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AA7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AB7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AC7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AE7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AF7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AG7" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AH7" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AI7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AJ7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AK7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AL7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AM7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AN7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AO7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AP7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AQ7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AR7" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AS7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AT7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AU7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AV7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AW7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AX7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AY7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AZ7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BA7" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BB7" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8" spans="1:54" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="D8" s="3">
         <v>25</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="M8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="R8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="S8" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="V8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="X8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AB8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AC8" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD8" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AF8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AG8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AH8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AI8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AJ8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AK8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AL8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AM8" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AN8" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AO8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AP8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AQ8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AR8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AS8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AT8" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AU8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AV8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AW8" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AX8" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AY8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AZ8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BA8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BB8" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:54" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D9" s="3">
         <v>20</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="K9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T9" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="U9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Z9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AA9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AB9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AC9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AD9" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AE9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AJ9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AK9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AL9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AM9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AN9" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AO9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AP9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AQ9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AR9" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AS9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AT9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AU9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AV9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AW9" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AX9" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AY9" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AZ9" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BA9" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BB9" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:54" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="D10" s="3">
         <v>10</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M10" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P10" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V10" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W10" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="X10" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Y10" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z10" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA10" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AB10" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AC10" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD10" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AE10" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AF10" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AG10" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AH10" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AI10" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AJ10" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AK10" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AL10" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AM10" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AN10" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AO10" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AP10" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AQ10" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AR10" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AS10" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AT10" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AU10" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AV10" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AW10" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AX10" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AY10" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AZ10" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BA10" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="BB10" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:54" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>55</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>56</v>
       </c>
       <c r="D11" s="3">
         <v>12</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="I11" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="J11" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N11" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q11" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R11" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="S11" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="T11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="U11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="V11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="W11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X11" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y11" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z11" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AA11" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AB11" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AC11" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AD11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AE11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AF11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AG11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH11" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AI11" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AJ11" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AK11" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AL11" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AM11" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AN11" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AO11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AP11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AQ11" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AR11" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AS11" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AT11" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AU11" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AV11" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AW11" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AX11" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AY11" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AZ11" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BA11" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BB11" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:54" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="D12" s="3">
         <v>14</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J12" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K12" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L12" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="N12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O12" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="P12" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Q12" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R12" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S12" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="U12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="V12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="X12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y12" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="Z12" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AA12" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AB12" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC12" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AE12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AF12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AG12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AH12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AI12" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AJ12" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AK12" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL12" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM12" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AN12" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AO12" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AP12" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AQ12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AR12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AS12" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AT12" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AU12" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AV12" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AW12" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AX12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AY12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AZ12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BA12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BB12" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:54" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D13" s="3">
         <v>9</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I13" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="J13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="N13" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P13" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q13" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="R13" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S13" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="T13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="U13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="V13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="W13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="X13" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="Y13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Z13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AA13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AB13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AC13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AD13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AE13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AF13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AG13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AH13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AI13" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AJ13" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AK13" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AL13" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM13" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AN13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AO13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AP13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AQ13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AR13" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AS13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AT13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AU13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AV13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AW13" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AX13" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AY13" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AZ13" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BA13" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BB13" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="14" spans="1:54" ht="65.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D14" s="3">
         <v>8</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G14" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="M14" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="N14" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O14" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P14" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Q14" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="R14" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S14" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="T14" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="U14" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="V14" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="W14" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="X14" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y14" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="Z14" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AA14" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AB14" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AC14" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AD14" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AE14" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AF14" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AG14" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AH14" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AI14" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AJ14" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AK14" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AL14" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AM14" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AN14" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AO14" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AP14" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AQ14" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AR14" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AS14" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AT14" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AU14" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AV14" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AW14" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AX14" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AY14" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AZ14" s="5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="BA14" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="BB14" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>